<commit_message>
feat: complete auth flow and project management, add gh-pages deploy config
</commit_message>
<xml_diff>
--- a/requirements/作物表型数据采集表_定稿_20260110.xlsx
+++ b/requirements/作物表型数据采集表_定稿_20260110.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jianchaoci/app_developments/deci_data_collection/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E4A75E-EC3A-6D43-A9B1-C47ABB282847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5073EE-70A2-6346-BC1C-AE7F0F3C49FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="620" windowWidth="22420" windowHeight="25300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4720" yWindow="3060" windowWidth="34980" windowHeight="25300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="番茄" sheetId="1" r:id="rId1"/>
@@ -144,9 +144,6 @@
     <t>可溶性固形物（糖）</t>
   </si>
   <si>
-    <t>酸度</t>
-  </si>
-  <si>
     <t>灌溉量（天）</t>
   </si>
   <si>
@@ -166,15 +163,6 @@
   </si>
   <si>
     <t>灌溉pH（天）</t>
-  </si>
-  <si>
-    <t>每天产量（天）</t>
-  </si>
-  <si>
-    <t>单周产量（天）</t>
-  </si>
-  <si>
-    <t>报损量</t>
   </si>
   <si>
     <t>单位</t>
@@ -456,6 +444,22 @@
   </si>
   <si>
     <t>单位产量（天）</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>每天产量（天）</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>酸度</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>单周产量（天）</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>报损量</t>
     <phoneticPr fontId="17" type="noConversion"/>
   </si>
 </sst>
@@ -821,7 +825,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1048,9 +1052,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1540,10 +1541,10 @@
   <dimension ref="A1:AF36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="P5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AE4" sqref="AE4"/>
+      <selection pane="bottomRight" activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.5" customHeight="1"/>
@@ -1719,16 +1720,16 @@
         <v>21</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="M4" s="20" t="s">
         <v>22</v>
@@ -1740,126 +1741,126 @@
         <v>24</v>
       </c>
       <c r="P4" s="20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Q4" s="20" t="s">
         <v>25</v>
       </c>
       <c r="R4" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="S4" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="S4" s="22" t="s">
+      <c r="T4" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="T4" s="20" t="s">
+      <c r="U4" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="V4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="U4" s="20" t="s">
+      <c r="W4" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="X4" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y4" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z4" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA4" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB4" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="AC4" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="V4" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="W4" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="X4" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y4" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z4" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA4" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB4" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC4" s="23" t="s">
-        <v>124</v>
-      </c>
       <c r="AD4" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE4" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="AE4" s="23" t="s">
+      <c r="AF4" s="20" t="s">
         <v>125</v>
-      </c>
-      <c r="AF4" s="20" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="23.25" customHeight="1">
       <c r="A5" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="H5" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="N5" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q5" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="R5" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="S5" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="24" t="s">
+      <c r="T5" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="U5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="V5" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" s="24" t="s">
+      <c r="W5" s="31" t="s">
         <v>42</v>
-      </c>
-      <c r="N5" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="P5" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q5" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="R5" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="S5" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="T5" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="U5" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="V5" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="W5" s="31" t="s">
-        <v>46</v>
       </c>
       <c r="X5" s="24">
         <f>-X11</f>
@@ -1869,218 +1870,218 @@
       <c r="Z5" s="24"/>
       <c r="AA5" s="32"/>
       <c r="AB5" s="30" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="AC5" s="30" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="AD5" s="30" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="AE5" s="30"/>
       <c r="AF5" s="22" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="157.5" customHeight="1">
       <c r="A6" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="F6" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="G6" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="H6" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="I6" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="K6" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="L6" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="N6" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6" s="30" t="s">
+      <c r="O6" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="K6" s="24" t="s">
+      <c r="P6" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="L6" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="M6" s="24" t="s">
+      <c r="Q6" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="N6" s="24" t="s">
+      <c r="R6" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="O6" s="24" t="s">
+      <c r="S6" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="P6" s="30" t="s">
+      <c r="T6" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="Q6" s="24" t="s">
+      <c r="U6" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="R6" s="29" t="s">
+      <c r="V6" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="S6" s="24" t="s">
+      <c r="W6" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="T6" s="24" t="s">
+      <c r="X6" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="U6" s="30" t="s">
+      <c r="Y6" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="V6" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="W6" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="X6" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y6" s="24" t="s">
-        <v>72</v>
-      </c>
       <c r="Z6" s="24" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AA6" s="34" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="AB6" s="30" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="AC6" s="30" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AD6" s="30" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="AE6" s="30" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AF6" s="35" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:32" ht="73.5" customHeight="1">
       <c r="A7" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="K7" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="L7" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="M7" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="N7" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="O7" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="P7" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q7" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="R7" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="S7" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="T7" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="U7" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="V7" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="W7" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="X7" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y7" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z7" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA7" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB7" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC7" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="AD7" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE7" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="F7" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="G7" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="H7" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="I7" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="J7" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="K7" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="L7" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="M7" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="N7" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="O7" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="P7" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q7" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="R7" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="S7" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="T7" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="U7" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="V7" s="42" t="s">
-        <v>122</v>
-      </c>
-      <c r="W7" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="X7" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y7" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z7" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA7" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB7" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="AC7" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="AD7" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="AE7" s="44" t="s">
-        <v>78</v>
-      </c>
       <c r="AF7" s="45" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:32" ht="114.5" customHeight="1">
       <c r="A8" s="36" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B8" s="37"/>
       <c r="C8" s="46"/>
@@ -2090,30 +2091,30 @@
       <c r="G8" s="37"/>
       <c r="H8" s="47"/>
       <c r="I8" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="N8" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="O8" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="J8" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="K8" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="N8" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="O8" s="50" t="s">
-        <v>84</v>
-      </c>
       <c r="P8" s="50" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="R8" s="11"/>
       <c r="AA8" s="43"/>
       <c r="AB8" s="49" t="s">
-        <v>85</v>
-      </c>
-      <c r="AC8" s="76" t="s">
-        <v>119</v>
+        <v>81</v>
+      </c>
+      <c r="AC8" s="30" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:32" ht="120" customHeight="1">
@@ -2129,16 +2130,16 @@
       <c r="H9" s="47"/>
       <c r="I9" s="37"/>
       <c r="J9" s="51" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="K9" s="37" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="O9" s="24" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="P9" s="52" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="R9" s="11"/>
     </row>
@@ -2580,25 +2581,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17">
       <c r="A1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17">
@@ -2606,13 +2607,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="73" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E2" s="3">
         <v>50</v>
@@ -2621,7 +2622,7 @@
         <v>500</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17">
@@ -2630,10 +2631,10 @@
       </c>
       <c r="B3" s="74"/>
       <c r="C3" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E3" s="3">
         <v>50</v>
@@ -2642,7 +2643,7 @@
         <v>1000</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="51">
@@ -2656,7 +2657,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E4" s="3">
         <v>5</v>
@@ -2665,7 +2666,7 @@
         <v>30</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="34">
@@ -2676,10 +2677,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E5" s="3">
         <v>5</v>
@@ -2688,7 +2689,7 @@
         <v>60</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="51">
@@ -2697,10 +2698,10 @@
       </c>
       <c r="B6" s="75"/>
       <c r="C6" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E6" s="3">
         <v>5</v>
@@ -2709,7 +2710,7 @@
         <v>30</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="51">
@@ -2718,10 +2719,10 @@
       </c>
       <c r="B7" s="75"/>
       <c r="C7" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E7" s="3">
         <v>3</v>
@@ -2730,7 +2731,7 @@
         <v>20</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="68">
@@ -2739,10 +2740,10 @@
       </c>
       <c r="B8" s="75"/>
       <c r="C8" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E8" s="3">
         <v>5</v>
@@ -2751,7 +2752,7 @@
         <v>20</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="68">
@@ -2760,10 +2761,10 @@
       </c>
       <c r="B9" s="74"/>
       <c r="C9" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E9" s="3">
         <v>5</v>
@@ -2772,7 +2773,7 @@
         <v>20</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2786,21 +2787,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000C69FA04A46F646B9C46410CE814DDF" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4b6e38c3db47db8271e20bb9b0485729">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="763d3d30-2c9f-4a07-a3c7-72c861f4b359" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a6ad8efe43623f9de79994a908457434" ns2:_="">
     <xsd:import namespace="763d3d30-2c9f-4a07-a3c7-72c861f4b359"/>
@@ -2938,8 +2924,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69D92C0A-BEC3-4C42-A5A0-77E81BAE23CC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE58AAAF-7AD3-4404-8D24-7DB1B31C6CA5}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
@@ -2951,7 +2952,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE58AAAF-7AD3-4404-8D24-7DB1B31C6CA5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69D92C0A-BEC3-4C42-A5A0-77E81BAE23CC}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>